<commit_message>
Added components from bootstrap to make the website look and feel a lot nicer, it's still far from perfect though
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28401F84-9EC1-458E-B796-A90899860A30}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951FF101-019A-4968-8ACB-688F802DF337}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="1" xr2:uid="{58DD74EF-95EE-4947-B358-20B5CBB4703D}"/>
+    <workbookView xWindow="4695" yWindow="3180" windowWidth="20910" windowHeight="11835" xr2:uid="{58DD74EF-95EE-4947-B358-20B5CBB4703D}"/>
   </bookViews>
   <sheets>
     <sheet name="NCES Data By Major" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'List Of US Colleges'!$B$2:$B$1976</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'NCES Data By Major'!$C$2:$F$155</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'NCES Data By Major'!$C$2:$F$157</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="2103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="2105">
   <si>
     <t>Agriculture</t>
   </si>
@@ -6346,6 +6346,12 @@
   </si>
   <si>
     <t>Youngstown State University</t>
+  </si>
+  <si>
+    <t>Journalism</t>
+  </si>
+  <si>
+    <t>Radio</t>
   </si>
 </sst>
 </file>
@@ -6817,10 +6823,10 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="B2:F155"/>
+  <dimension ref="B2:F157"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A139" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8399,16 +8405,16 @@
         <v>92</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>148</v>
+        <v>2103</v>
       </c>
       <c r="D94" s="9">
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="E94" s="10">
-        <v>1.2E-2</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="F94" s="2">
-        <v>42000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.25">
@@ -8416,16 +8422,16 @@
         <v>93</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>74</v>
+        <v>148</v>
       </c>
       <c r="D95" s="9">
-        <v>7.2000000000000008E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="E95" s="10">
         <v>1.2E-2</v>
       </c>
       <c r="F95" s="2">
-        <v>39000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.25">
@@ -8433,16 +8439,16 @@
         <v>94</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D96" s="9">
-        <v>8.5999999999999993E-2</v>
+        <v>7.2000000000000008E-2</v>
       </c>
       <c r="E96" s="10">
-        <v>1.7000000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F96" s="2">
-        <v>45000</v>
+        <v>39000</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
@@ -8450,16 +8456,16 @@
         <v>95</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>144</v>
+        <v>75</v>
       </c>
       <c r="D97" s="9">
-        <v>7.8E-2</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="E97" s="10">
-        <v>1.6E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="F97" s="2">
-        <v>42000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
@@ -8467,16 +8473,16 @@
         <v>96</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="D98" s="9">
-        <v>8.199999999999999E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="E98" s="10">
-        <v>0.01</v>
+        <v>1.6E-2</v>
       </c>
       <c r="F98" s="2">
-        <v>65000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
@@ -8484,16 +8490,16 @@
         <v>97</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="D99" s="9">
-        <v>6.5000000000000002E-2</v>
+        <v>8.199999999999999E-2</v>
       </c>
       <c r="E99" s="10">
-        <v>6.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F99" s="2">
-        <v>50000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
@@ -8501,16 +8507,16 @@
         <v>98</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D100" s="9">
-        <v>3.4000000000000002E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E100" s="10">
-        <v>1.1000000000000001E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F100" s="2">
-        <v>66000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
@@ -8518,16 +8524,16 @@
         <v>99</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="D101" s="9">
-        <v>4.9000000000000002E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E101" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="F101" s="2">
-        <v>49000</v>
+        <v>66000</v>
       </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
@@ -8535,16 +8541,16 @@
         <v>100</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="D102" s="9">
-        <v>4.5999999999999999E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E102" s="10">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F102" s="2">
-        <v>50000</v>
+        <v>49000</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
@@ -8552,7 +8558,7 @@
         <v>101</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D103" s="9">
         <v>4.5999999999999999E-2</v>
@@ -8569,16 +8575,16 @@
         <v>102</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>103</v>
+        <v>27</v>
       </c>
       <c r="D104" s="9">
-        <v>8.199999999999999E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="E104" s="10">
-        <v>0.01</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F104" s="2">
-        <v>65000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
@@ -8586,16 +8592,16 @@
         <v>103</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>6</v>
+        <v>103</v>
       </c>
       <c r="D105" s="9">
-        <v>4.5999999999999999E-2</v>
+        <v>8.199999999999999E-2</v>
       </c>
       <c r="E105" s="10">
         <v>0.01</v>
       </c>
       <c r="F105" s="2">
-        <v>55000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
@@ -8603,16 +8609,16 @@
         <v>104</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="D106" s="9">
-        <v>3.7000000000000005E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="E106" s="10">
-        <v>8.0000000000000002E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F106" s="2">
-        <v>72000</v>
+        <v>55000</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.25">
@@ -8620,16 +8626,16 @@
         <v>105</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>154</v>
+        <v>60</v>
       </c>
       <c r="D107" s="9">
-        <v>6.8000000000000005E-2</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="E107" s="10">
-        <v>6.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F107" s="2">
-        <v>40000</v>
+        <v>72000</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.25">
@@ -8637,16 +8643,16 @@
         <v>106</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>33</v>
+        <v>154</v>
       </c>
       <c r="D108" s="9">
-        <v>4.4999999999999998E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="E108" s="10">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="F108" s="2">
-        <v>51000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.25">
@@ -8654,16 +8660,16 @@
         <v>107</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>121</v>
+        <v>33</v>
       </c>
       <c r="D109" s="9">
-        <v>4.9000000000000002E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E109" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F109" s="2">
-        <v>49000</v>
+        <v>51000</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.25">
@@ -8671,16 +8677,16 @@
         <v>108</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="D110" s="9">
-        <v>8.199999999999999E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E110" s="10">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F110" s="2">
-        <v>65000</v>
+        <v>49000</v>
       </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
@@ -8688,16 +8694,16 @@
         <v>109</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D111" s="9">
-        <v>3.9E-2</v>
+        <v>8.199999999999999E-2</v>
       </c>
       <c r="E111" s="10">
-        <v>1.9E-2</v>
+        <v>0.01</v>
       </c>
       <c r="F111" s="2">
-        <v>35000</v>
+        <v>65000</v>
       </c>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
@@ -8705,16 +8711,16 @@
         <v>110</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="D112" s="9">
-        <v>4.7E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="E112" s="10">
-        <v>8.0000000000000002E-3</v>
+        <v>1.9E-2</v>
       </c>
       <c r="F112" s="2">
-        <v>48000</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
@@ -8722,16 +8728,16 @@
         <v>111</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D113" s="9">
-        <v>5.4000000000000006E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="E113" s="10">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F113" s="2">
-        <v>45000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
@@ -8739,16 +8745,16 @@
         <v>112</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
       <c r="D114" s="9">
-        <v>6.8000000000000005E-2</v>
+        <v>5.4000000000000006E-2</v>
       </c>
       <c r="E114" s="10">
-        <v>6.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F114" s="2">
-        <v>40000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
@@ -8756,16 +8762,16 @@
         <v>113</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D115" s="9">
-        <v>5.2000000000000005E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="E115" s="10">
-        <v>4.0000000000000001E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F115" s="2">
-        <v>48000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.25">
@@ -8773,16 +8779,16 @@
         <v>114</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="D116" s="9">
-        <v>4.9000000000000002E-2</v>
+        <v>5.2000000000000005E-2</v>
       </c>
       <c r="E116" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F116" s="2">
-        <v>49000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
@@ -8790,7 +8796,7 @@
         <v>115</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D117" s="9">
         <v>4.9000000000000002E-2</v>
@@ -8807,16 +8813,16 @@
         <v>116</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>4</v>
+        <v>126</v>
       </c>
       <c r="D118" s="9">
-        <v>0.03</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E118" s="10">
-        <v>6.0000000000000001E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F118" s="2">
-        <v>57000</v>
+        <v>49000</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.25">
@@ -8824,16 +8830,16 @@
         <v>117</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>117</v>
+        <v>4</v>
       </c>
       <c r="D119" s="9">
-        <v>0.09</v>
+        <v>0.03</v>
       </c>
       <c r="E119" s="10">
-        <v>2.3E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F119" s="2">
-        <v>40000</v>
+        <v>57000</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.25">
@@ -8841,16 +8847,16 @@
         <v>118</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="D120" s="9">
-        <v>6.2E-2</v>
+        <v>0.09</v>
       </c>
       <c r="E120" s="10">
-        <v>6.9999999999999993E-3</v>
+        <v>2.3E-2</v>
       </c>
       <c r="F120" s="2">
-        <v>42000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.25">
@@ -8858,10 +8864,10 @@
         <v>119</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D121" s="9">
-        <v>3.5000000000000003E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="E121" s="10">
         <v>6.9999999999999993E-3</v>
@@ -8875,16 +8881,16 @@
         <v>120</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="D122" s="9">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E122" s="10">
-        <v>6.0000000000000001E-3</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="F122" s="2">
-        <v>57000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.25">
@@ -8892,7 +8898,7 @@
         <v>121</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D123" s="9">
         <v>0.03</v>
@@ -8909,16 +8915,16 @@
         <v>122</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="D124" s="9">
-        <v>7.8E-2</v>
+        <v>0.03</v>
       </c>
       <c r="E124" s="10">
-        <v>1.6E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F124" s="2">
-        <v>42000</v>
+        <v>57000</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.25">
@@ -8926,16 +8932,16 @@
         <v>123</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="D125" s="9">
-        <v>4.7E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="E125" s="10">
-        <v>8.0000000000000002E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="F125" s="2">
-        <v>48000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.25">
@@ -8943,16 +8949,16 @@
         <v>124</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D126" s="9">
-        <v>3.5000000000000003E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="E126" s="10">
-        <v>6.9999999999999993E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F126" s="2">
-        <v>42000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.25">
@@ -8960,16 +8966,16 @@
         <v>125</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D127" s="9">
-        <v>4.7E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E127" s="10">
-        <v>8.0000000000000002E-3</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="F127" s="2">
-        <v>48000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="128" spans="2:6" x14ac:dyDescent="0.25">
@@ -8977,7 +8983,7 @@
         <v>126</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="D128" s="9">
         <v>4.7E-2</v>
@@ -8994,16 +9000,16 @@
         <v>127</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>124</v>
+        <v>84</v>
       </c>
       <c r="D129" s="9">
-        <v>4.9000000000000002E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="E129" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="F129" s="2">
-        <v>49000</v>
+        <v>48000</v>
       </c>
     </row>
     <row r="130" spans="2:6" x14ac:dyDescent="0.25">
@@ -9011,16 +9017,16 @@
         <v>128</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D130" s="9">
-        <v>5.9000000000000004E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E130" s="10">
-        <v>6.9999999999999993E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F130" s="2">
-        <v>50000</v>
+        <v>49000</v>
       </c>
     </row>
     <row r="131" spans="2:6" x14ac:dyDescent="0.25">
@@ -9028,16 +9034,16 @@
         <v>129</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="D131" s="9">
-        <v>4.5999999999999999E-2</v>
+        <v>5.9000000000000004E-2</v>
       </c>
       <c r="E131" s="10">
-        <v>0.01</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="F131" s="2">
-        <v>55000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="132" spans="2:6" x14ac:dyDescent="0.25">
@@ -9045,16 +9051,16 @@
         <v>130</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>9</v>
+        <v>140</v>
       </c>
       <c r="D132" s="9">
-        <v>5.9000000000000004E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="E132" s="10">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F132" s="2">
-        <v>40000</v>
+        <v>55000</v>
       </c>
     </row>
     <row r="133" spans="2:6" x14ac:dyDescent="0.25">
@@ -9062,16 +9068,16 @@
         <v>131</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="D133" s="9">
-        <v>0.09</v>
+        <v>5.9000000000000004E-2</v>
       </c>
       <c r="E133" s="10">
-        <v>2.3E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F133" s="2">
-        <v>45000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="134" spans="2:6" x14ac:dyDescent="0.25">
@@ -9079,16 +9085,16 @@
         <v>132</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="D134" s="9">
-        <v>4.4999999999999998E-2</v>
+        <v>0.09</v>
       </c>
       <c r="E134" s="10">
-        <v>6.0000000000000001E-3</v>
+        <v>2.3E-2</v>
       </c>
       <c r="F134" s="2">
-        <v>51000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="135" spans="2:6" x14ac:dyDescent="0.25">
@@ -9096,16 +9102,16 @@
         <v>133</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="D135" s="9">
-        <v>0.09</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E135" s="10">
-        <v>2.3E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F135" s="2">
-        <v>45000</v>
+        <v>51000</v>
       </c>
     </row>
     <row r="136" spans="2:6" x14ac:dyDescent="0.25">
@@ -9113,16 +9119,16 @@
         <v>134</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="D136" s="9">
-        <v>4.9000000000000002E-2</v>
+        <v>0.09</v>
       </c>
       <c r="E136" s="10">
-        <v>6.0000000000000001E-3</v>
+        <v>2.3E-2</v>
       </c>
       <c r="F136" s="2">
-        <v>64000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="137" spans="2:6" x14ac:dyDescent="0.25">
@@ -9130,16 +9136,16 @@
         <v>135</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>152</v>
+        <v>38</v>
       </c>
       <c r="D137" s="9">
-        <v>5.7999999999999996E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E137" s="10">
-        <v>6.9999999999999993E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F137" s="2">
-        <v>58000</v>
+        <v>64000</v>
       </c>
     </row>
     <row r="138" spans="2:6" x14ac:dyDescent="0.25">
@@ -9147,16 +9153,16 @@
         <v>136</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>114</v>
+        <v>2104</v>
       </c>
       <c r="D138" s="9">
-        <v>3.9E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="E138" s="10">
-        <v>1.9E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F138" s="2">
-        <v>35000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="139" spans="2:6" x14ac:dyDescent="0.25">
@@ -9164,16 +9170,16 @@
         <v>137</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="D139" s="9">
-        <v>7.8E-2</v>
+        <v>5.7999999999999996E-2</v>
       </c>
       <c r="E139" s="10">
-        <v>1.6E-2</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="F139" s="2">
-        <v>42000</v>
+        <v>58000</v>
       </c>
     </row>
     <row r="140" spans="2:6" x14ac:dyDescent="0.25">
@@ -9181,16 +9187,16 @@
         <v>138</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="D140" s="9">
-        <v>2.5000000000000001E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="E140" s="10">
-        <v>1.1000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="F140" s="2">
-        <v>42000</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="141" spans="2:6" x14ac:dyDescent="0.25">
@@ -9198,16 +9204,16 @@
         <v>139</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="D141" s="9">
-        <v>6.9000000000000006E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="E141" s="10">
-        <v>4.0000000000000001E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="F141" s="2">
-        <v>50000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="142" spans="2:6" x14ac:dyDescent="0.25">
@@ -9215,13 +9221,13 @@
         <v>140</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>109</v>
+        <v>52</v>
       </c>
       <c r="D142" s="9">
-        <v>5.2999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="E142" s="10">
-        <v>1.3999999999999999E-2</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="F142" s="2">
         <v>42000</v>
@@ -9232,16 +9238,16 @@
         <v>141</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D143" s="9">
-        <v>5.5999999999999994E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="E143" s="10">
-        <v>1.3999999999999999E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F143" s="2">
-        <v>38000</v>
+        <v>50000</v>
       </c>
     </row>
     <row r="144" spans="2:6" x14ac:dyDescent="0.25">
@@ -9249,13 +9255,13 @@
         <v>142</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="D144" s="9">
-        <v>7.5999999999999998E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="E144" s="10">
-        <v>1.2E-2</v>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="F144" s="2">
         <v>42000</v>
@@ -9266,16 +9272,16 @@
         <v>143</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D145" s="9">
-        <v>3.5000000000000003E-2</v>
+        <v>5.5999999999999994E-2</v>
       </c>
       <c r="E145" s="10">
-        <v>6.9999999999999993E-3</v>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="F145" s="2">
-        <v>42000</v>
+        <v>38000</v>
       </c>
     </row>
     <row r="146" spans="2:6" x14ac:dyDescent="0.25">
@@ -9283,16 +9289,16 @@
         <v>144</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="D146" s="9">
-        <v>3.4000000000000002E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="E146" s="10">
-        <v>1.1000000000000001E-2</v>
+        <v>1.2E-2</v>
       </c>
       <c r="F146" s="2">
-        <v>66000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="147" spans="2:6" x14ac:dyDescent="0.25">
@@ -9300,16 +9306,16 @@
         <v>145</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="D147" s="9">
-        <v>4.9000000000000002E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E147" s="10">
-        <v>0.01</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="F147" s="2">
-        <v>70000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="148" spans="2:6" x14ac:dyDescent="0.25">
@@ -9317,16 +9323,16 @@
         <v>146</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>155</v>
+        <v>31</v>
       </c>
       <c r="D148" s="9">
-        <v>6.8000000000000005E-2</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E148" s="10">
-        <v>6.0000000000000001E-3</v>
+        <v>1.1000000000000001E-2</v>
       </c>
       <c r="F148" s="2">
-        <v>40000</v>
+        <v>66000</v>
       </c>
     </row>
     <row r="149" spans="2:6" x14ac:dyDescent="0.25">
@@ -9334,16 +9340,16 @@
         <v>147</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D149" s="9">
-        <v>6.8000000000000005E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E149" s="10">
-        <v>6.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="F149" s="2">
-        <v>40000</v>
+        <v>70000</v>
       </c>
     </row>
     <row r="150" spans="2:6" x14ac:dyDescent="0.25">
@@ -9351,16 +9357,16 @@
         <v>148</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="D150" s="9">
-        <v>3.9E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="E150" s="10">
-        <v>1.9E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F150" s="2">
-        <v>35000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="151" spans="2:6" x14ac:dyDescent="0.25">
@@ -9368,16 +9374,16 @@
         <v>149</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>41</v>
+        <v>150</v>
       </c>
       <c r="D151" s="9">
-        <v>4.8000000000000001E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="E151" s="10">
-        <v>1.6E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="F151" s="2">
-        <v>59000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="152" spans="2:6" x14ac:dyDescent="0.25">
@@ -9385,16 +9391,16 @@
         <v>150</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="D152" s="9">
-        <v>3.5000000000000003E-2</v>
+        <v>3.9E-2</v>
       </c>
       <c r="E152" s="10">
-        <v>6.9999999999999993E-3</v>
+        <v>1.9E-2</v>
       </c>
       <c r="F152" s="2">
-        <v>42000</v>
+        <v>35000</v>
       </c>
     </row>
     <row r="153" spans="2:6" x14ac:dyDescent="0.25">
@@ -9402,16 +9408,16 @@
         <v>151</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="D153" s="9">
-        <v>0.09</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="E153" s="10">
-        <v>2.3E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="F153" s="2">
-        <v>40000</v>
+        <v>59000</v>
       </c>
     </row>
     <row r="154" spans="2:6" x14ac:dyDescent="0.25">
@@ -9419,16 +9425,16 @@
         <v>152</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D154" s="9">
-        <v>4.4999999999999998E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E154" s="10">
-        <v>1.1000000000000001E-2</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="F154" s="2">
-        <v>41000</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="155" spans="2:6" x14ac:dyDescent="0.25">
@@ -9436,25 +9442,59 @@
         <v>153</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="D155" s="9">
-        <v>7.5999999999999998E-2</v>
+        <v>0.09</v>
       </c>
       <c r="E155" s="10">
-        <v>6.9999999999999993E-3</v>
+        <v>2.3E-2</v>
       </c>
       <c r="F155" s="2">
         <v>40000</v>
       </c>
     </row>
+    <row r="156" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B156" s="8">
+        <v>154</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D156" s="9">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E156" s="10">
+        <v>1.1000000000000001E-2</v>
+      </c>
+      <c r="F156" s="2">
+        <v>41000</v>
+      </c>
+    </row>
+    <row r="157" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B157" s="8">
+        <v>155</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D157" s="9">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E157" s="10">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="F157" s="2">
+        <v>40000</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C2:F155" xr:uid="{17FFB986-A331-43CB-ACB0-C247D92CA52A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:F155">
-      <sortCondition ref="C2:C155"/>
+  <autoFilter ref="C2:F157" xr:uid="{17FFB986-A331-43CB-ACB0-C247D92CA52A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C3:F157">
+      <sortCondition ref="C2:C157"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="C3:C155">
+  <conditionalFormatting sqref="C3:C157">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9468,7 +9508,7 @@
   </sheetPr>
   <dimension ref="B2:B1976"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -19727,499 +19767,499 @@
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C61&amp;""", medianIncome: "&amp;'NCES Data By Major'!F61&amp;" } ,"</f>
-        <v>{ description: "English Literature", medianIncome: 40000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C62&amp;""", medianIncome: "&amp;'NCES Data By Major'!F62&amp;" } ,"</f>
+        <v>{ description: "Environmental Science", medianIncome: 45000 } ,</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C62&amp;""", medianIncome: "&amp;'NCES Data By Major'!F62&amp;" } ,"</f>
-        <v>{ description: "Environmental Science", medianIncome: 45000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C63&amp;""", medianIncome: "&amp;'NCES Data By Major'!F63&amp;" } ,"</f>
+        <v>{ description: "Epidemiology", medianIncome: 51000 } ,</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C63&amp;""", medianIncome: "&amp;'NCES Data By Major'!F63&amp;" } ,"</f>
-        <v>{ description: "Epidemiology", medianIncome: 51000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C64&amp;""", medianIncome: "&amp;'NCES Data By Major'!F64&amp;" } ,"</f>
+        <v>{ description: "Ethnic Studies", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C64&amp;""", medianIncome: "&amp;'NCES Data By Major'!F64&amp;" } ,"</f>
-        <v>{ description: "Ethnic Studies", medianIncome: 42000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C65&amp;""", medianIncome: "&amp;'NCES Data By Major'!F65&amp;" } ,"</f>
+        <v>{ description: "Family Studies", medianIncome: 38000 } ,</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C65&amp;""", medianIncome: "&amp;'NCES Data By Major'!F65&amp;" } ,"</f>
-        <v>{ description: "Family Studies", medianIncome: 38000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C66&amp;""", medianIncome: "&amp;'NCES Data By Major'!F66&amp;" } ,"</f>
+        <v>{ description: "Finance", medianIncome: 64000 } ,</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C66&amp;""", medianIncome: "&amp;'NCES Data By Major'!F66&amp;" } ,"</f>
-        <v>{ description: "Finance", medianIncome: 64000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C67&amp;""", medianIncome: "&amp;'NCES Data By Major'!F67&amp;" } ,"</f>
+        <v>{ description: "Fine Arts", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C67&amp;""", medianIncome: "&amp;'NCES Data By Major'!F67&amp;" } ,"</f>
-        <v>{ description: "Fine Arts", medianIncome: 40000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C68&amp;""", medianIncome: "&amp;'NCES Data By Major'!F68&amp;" } ,"</f>
+        <v>{ description: "Fire Protection", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C68&amp;""", medianIncome: "&amp;'NCES Data By Major'!F68&amp;" } ,"</f>
-        <v>{ description: "Fire Protection", medianIncome: 42000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C69&amp;""", medianIncome: "&amp;'NCES Data By Major'!F69&amp;" } ,"</f>
+        <v>{ description: "Foreign Language(s)", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C69&amp;""", medianIncome: "&amp;'NCES Data By Major'!F69&amp;" } ,"</f>
-        <v>{ description: "Foreign Language(s)", medianIncome: 40000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C70&amp;""", medianIncome: "&amp;'NCES Data By Major'!F70&amp;" } ,"</f>
+        <v>{ description: "Foreign Literature", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C70&amp;""", medianIncome: "&amp;'NCES Data By Major'!F70&amp;" } ,"</f>
-        <v>{ description: "Foreign Literature", medianIncome: 40000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C71&amp;""", medianIncome: "&amp;'NCES Data By Major'!F71&amp;" } ,"</f>
+        <v>{ description: "Forensics", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C71&amp;""", medianIncome: "&amp;'NCES Data By Major'!F71&amp;" } ,"</f>
-        <v>{ description: "Forensics", medianIncome: 42000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C72&amp;""", medianIncome: "&amp;'NCES Data By Major'!F72&amp;" } ,"</f>
+        <v>{ description: "Gender Studies", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C72&amp;""", medianIncome: "&amp;'NCES Data By Major'!F72&amp;" } ,"</f>
-        <v>{ description: "Gender Studies", medianIncome: 42000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C73&amp;""", medianIncome: "&amp;'NCES Data By Major'!F73&amp;" } ,"</f>
+        <v>{ description: "General Education", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C73&amp;""", medianIncome: "&amp;'NCES Data By Major'!F73&amp;" } ,"</f>
-        <v>{ description: "General Education", medianIncome: 40000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C74&amp;""", medianIncome: "&amp;'NCES Data By Major'!F74&amp;" } ,"</f>
+        <v>{ description: "General Engineering", medianIncome: 62000 } ,</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C74&amp;""", medianIncome: "&amp;'NCES Data By Major'!F74&amp;" } ,"</f>
-        <v>{ description: "General Engineering", medianIncome: 62000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C75&amp;""", medianIncome: "&amp;'NCES Data By Major'!F75&amp;" } ,"</f>
+        <v>{ description: "General Medical Services", medianIncome: 50000 } ,</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C75&amp;""", medianIncome: "&amp;'NCES Data By Major'!F75&amp;" } ,"</f>
-        <v>{ description: "General Medical Services", medianIncome: 50000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C76&amp;""", medianIncome: "&amp;'NCES Data By Major'!F76&amp;" } ,"</f>
+        <v>{ description: "Geography", medianIncome: 48000 } ,</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C76&amp;""", medianIncome: "&amp;'NCES Data By Major'!F76&amp;" } ,"</f>
-        <v>{ description: "Geography", medianIncome: 48000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C77&amp;""", medianIncome: "&amp;'NCES Data By Major'!F77&amp;" } ,"</f>
+        <v>{ description: "Geology", medianIncome: 45000 } ,</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C77&amp;""", medianIncome: "&amp;'NCES Data By Major'!F77&amp;" } ,"</f>
-        <v>{ description: "Geology", medianIncome: 45000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C78&amp;""", medianIncome: "&amp;'NCES Data By Major'!F78&amp;" } ,"</f>
+        <v>{ description: "Government", medianIncome: 50000 } ,</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C78&amp;""", medianIncome: "&amp;'NCES Data By Major'!F78&amp;" } ,"</f>
-        <v>{ description: "Government", medianIncome: 50000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C79&amp;""", medianIncome: "&amp;'NCES Data By Major'!F79&amp;" } ,"</f>
+        <v>{ description: "Graphic Design", medianIncome: 44000 } ,</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C79&amp;""", medianIncome: "&amp;'NCES Data By Major'!F79&amp;" } ,"</f>
-        <v>{ description: "Graphic Design", medianIncome: 44000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C80&amp;""", medianIncome: "&amp;'NCES Data By Major'!F80&amp;" } ,"</f>
+        <v>{ description: "Health Profession, Other", medianIncome: 54000 } ,</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C80&amp;""", medianIncome: "&amp;'NCES Data By Major'!F80&amp;" } ,"</f>
-        <v>{ description: "Health Profession, Other", medianIncome: 54000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C81&amp;""", medianIncome: "&amp;'NCES Data By Major'!F81&amp;" } ,"</f>
+        <v>{ description: "Health Services", medianIncome: 50000 } ,</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C81&amp;""", medianIncome: "&amp;'NCES Data By Major'!F81&amp;" } ,"</f>
-        <v>{ description: "Health Services", medianIncome: 50000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C82&amp;""", medianIncome: "&amp;'NCES Data By Major'!F82&amp;" } ,"</f>
+        <v>{ description: "History", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C82&amp;""", medianIncome: "&amp;'NCES Data By Major'!F82&amp;" } ,"</f>
-        <v>{ description: "History", medianIncome: 42000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C83&amp;""", medianIncome: "&amp;'NCES Data By Major'!F83&amp;" } ,"</f>
+        <v>{ description: "Home Economics", medianIncome: 38000 } ,</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C83&amp;""", medianIncome: "&amp;'NCES Data By Major'!F83&amp;" } ,"</f>
-        <v>{ description: "Home Economics", medianIncome: 38000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C84&amp;""", medianIncome: "&amp;'NCES Data By Major'!F84&amp;" } ,"</f>
+        <v>{ description: "Hospitality Services", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C84&amp;""", medianIncome: "&amp;'NCES Data By Major'!F84&amp;" } ,"</f>
-        <v>{ description: "Hospitality Services", medianIncome: 42000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C85&amp;""", medianIncome: "&amp;'NCES Data By Major'!F85&amp;" } ,"</f>
+        <v>{ description: "Hotel and Restaurant Management", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C85&amp;""", medianIncome: "&amp;'NCES Data By Major'!F85&amp;" } ,"</f>
-        <v>{ description: "Hotel and Restaurant Management", medianIncome: 42000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C86&amp;""", medianIncome: "&amp;'NCES Data By Major'!F86&amp;" } ,"</f>
+        <v>{ description: "Human Relations", medianIncome: 38000 } ,</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C86&amp;""", medianIncome: "&amp;'NCES Data By Major'!F86&amp;" } ,"</f>
-        <v>{ description: "Human Relations", medianIncome: 38000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C87&amp;""", medianIncome: "&amp;'NCES Data By Major'!F87&amp;" } ,"</f>
+        <v>{ description: "Human Services", medianIncome: 38000 } ,</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C87&amp;""", medianIncome: "&amp;'NCES Data By Major'!F87&amp;" } ,"</f>
-        <v>{ description: "Human Services", medianIncome: 38000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C88&amp;""", medianIncome: "&amp;'NCES Data By Major'!F88&amp;" } ,"</f>
+        <v>{ description: "Humanities", medianIncome: 39000 } ,</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C88&amp;""", medianIncome: "&amp;'NCES Data By Major'!F88&amp;" } ,"</f>
-        <v>{ description: "Humanities", medianIncome: 39000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C89&amp;""", medianIncome: "&amp;'NCES Data By Major'!F89&amp;" } ,"</f>
+        <v>{ description: "Information Science", medianIncome: 66000 } ,</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C89&amp;""", medianIncome: "&amp;'NCES Data By Major'!F89&amp;" } ,"</f>
-        <v>{ description: "Information Science", medianIncome: 66000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C90&amp;""", medianIncome: "&amp;'NCES Data By Major'!F90&amp;" } ,"</f>
+        <v>{ description: "Information Technology", medianIncome: 65000 } ,</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C90&amp;""", medianIncome: "&amp;'NCES Data By Major'!F90&amp;" } ,"</f>
-        <v>{ description: "Information Technology", medianIncome: 65000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C91&amp;""", medianIncome: "&amp;'NCES Data By Major'!F91&amp;" } ,"</f>
+        <v>{ description: "Insurance", medianIncome: 66000 } ,</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C91&amp;""", medianIncome: "&amp;'NCES Data By Major'!F91&amp;" } ,"</f>
-        <v>{ description: "Insurance", medianIncome: 66000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C92&amp;""", medianIncome: "&amp;'NCES Data By Major'!F92&amp;" } ,"</f>
+        <v>{ description: "Interdisciplinary Studies", medianIncome: 45000 } ,</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C92&amp;""", medianIncome: "&amp;'NCES Data By Major'!F92&amp;" } ,"</f>
-        <v>{ description: "Interdisciplinary Studies", medianIncome: 45000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C93&amp;""", medianIncome: "&amp;'NCES Data By Major'!F93&amp;" } ,"</f>
+        <v>{ description: "International Relations", medianIncome: 50000 } ,</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C93&amp;""", medianIncome: "&amp;'NCES Data By Major'!F93&amp;" } ,"</f>
-        <v>{ description: "International Relations", medianIncome: 50000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C94&amp;""", medianIncome: "&amp;'NCES Data By Major'!F94&amp;" } ,"</f>
+        <v>{ description: "Journalism", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C94&amp;""", medianIncome: "&amp;'NCES Data By Major'!F94&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C95&amp;""", medianIncome: "&amp;'NCES Data By Major'!F95&amp;" } ,"</f>
         <v>{ description: "Law", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C95&amp;""", medianIncome: "&amp;'NCES Data By Major'!F95&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C96&amp;""", medianIncome: "&amp;'NCES Data By Major'!F96&amp;" } ,"</f>
         <v>{ description: "Liberal Arts", medianIncome: 39000 } ,</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C96&amp;""", medianIncome: "&amp;'NCES Data By Major'!F96&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C97&amp;""", medianIncome: "&amp;'NCES Data By Major'!F97&amp;" } ,"</f>
         <v>{ description: "Linguistics", medianIncome: 45000 } ,</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C97&amp;""", medianIncome: "&amp;'NCES Data By Major'!F97&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C98&amp;""", medianIncome: "&amp;'NCES Data By Major'!F98&amp;" } ,"</f>
         <v>{ description: "Logic", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C98&amp;""", medianIncome: "&amp;'NCES Data By Major'!F98&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C99&amp;""", medianIncome: "&amp;'NCES Data By Major'!F99&amp;" } ,"</f>
         <v>{ description: "Macroeconomics", medianIncome: 65000 } ,</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C99&amp;""", medianIncome: "&amp;'NCES Data By Major'!F99&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C100&amp;""", medianIncome: "&amp;'NCES Data By Major'!F100&amp;" } ,"</f>
         <v>{ description: "Management and Administration", medianIncome: 50000 } ,</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C100&amp;""", medianIncome: "&amp;'NCES Data By Major'!F100&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C101&amp;""", medianIncome: "&amp;'NCES Data By Major'!F101&amp;" } ,"</f>
         <v>{ description: "Management Information Systems", medianIncome: 66000 } ,</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C101&amp;""", medianIncome: "&amp;'NCES Data By Major'!F101&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C102&amp;""", medianIncome: "&amp;'NCES Data By Major'!F102&amp;" } ,"</f>
         <v>{ description: "Marine Biology", medianIncome: 49000 } ,</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C102&amp;""", medianIncome: "&amp;'NCES Data By Major'!F102&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C103&amp;""", medianIncome: "&amp;'NCES Data By Major'!F103&amp;" } ,"</f>
         <v>{ description: "Marketing", medianIncome: 50000 } ,</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C103&amp;""", medianIncome: "&amp;'NCES Data By Major'!F103&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C104&amp;""", medianIncome: "&amp;'NCES Data By Major'!F104&amp;" } ,"</f>
         <v>{ description: "Marketing Research", medianIncome: 50000 } ,</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C104&amp;""", medianIncome: "&amp;'NCES Data By Major'!F104&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C105&amp;""", medianIncome: "&amp;'NCES Data By Major'!F105&amp;" } ,"</f>
         <v>{ description: "Mathematical Economics", medianIncome: 65000 } ,</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C105&amp;""", medianIncome: "&amp;'NCES Data By Major'!F105&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C106&amp;""", medianIncome: "&amp;'NCES Data By Major'!F106&amp;" } ,"</f>
         <v>{ description: "Mathematics", medianIncome: 55000 } ,</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C106&amp;""", medianIncome: "&amp;'NCES Data By Major'!F106&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C107&amp;""", medianIncome: "&amp;'NCES Data By Major'!F107&amp;" } ,"</f>
         <v>{ description: "Mechanical Engineering", medianIncome: 72000 } ,</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C107&amp;""", medianIncome: "&amp;'NCES Data By Major'!F107&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C108&amp;""", medianIncome: "&amp;'NCES Data By Major'!F108&amp;" } ,"</f>
         <v>{ description: "Media", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C108&amp;""", medianIncome: "&amp;'NCES Data By Major'!F108&amp;" } ,"</f>
-        <v>{ description: "Medical Administration", medianIncome: 51000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C110&amp;""", medianIncome: "&amp;'NCES Data By Major'!F110&amp;" } ,"</f>
+        <v>{ description: "Microbiology", medianIncome: 49000 } ,</v>
       </c>
     </row>
     <row r="109" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B109" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C109&amp;""", medianIncome: "&amp;'NCES Data By Major'!F109&amp;" } ,"</f>
-        <v>{ description: "Microbiology", medianIncome: 49000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C111&amp;""", medianIncome: "&amp;'NCES Data By Major'!F111&amp;" } ,"</f>
+        <v>{ description: "Microeconomics", medianIncome: 65000 } ,</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C110&amp;""", medianIncome: "&amp;'NCES Data By Major'!F110&amp;" } ,"</f>
-        <v>{ description: "Microeconomics", medianIncome: 65000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C112&amp;""", medianIncome: "&amp;'NCES Data By Major'!F112&amp;" } ,"</f>
+        <v>{ description: "Ministry", medianIncome: 35000 } ,</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C111&amp;""", medianIncome: "&amp;'NCES Data By Major'!F111&amp;" } ,"</f>
-        <v>{ description: "Ministry", medianIncome: 35000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C113&amp;""", medianIncome: "&amp;'NCES Data By Major'!F113&amp;" } ,"</f>
+        <v>{ description: "Molecular Biology", medianIncome: 48000 } ,</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C112&amp;""", medianIncome: "&amp;'NCES Data By Major'!F112&amp;" } ,"</f>
-        <v>{ description: "Molecular Biology", medianIncome: 48000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C114&amp;""", medianIncome: "&amp;'NCES Data By Major'!F114&amp;" } ,"</f>
+        <v>{ description: "Multidisciplinary Studies", medianIncome: 45000 } ,</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C113&amp;""", medianIncome: "&amp;'NCES Data By Major'!F113&amp;" } ,"</f>
-        <v>{ description: "Multidisciplinary Studies", medianIncome: 45000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C115&amp;""", medianIncome: "&amp;'NCES Data By Major'!F115&amp;" } ,"</f>
+        <v>{ description: "Music", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C114&amp;""", medianIncome: "&amp;'NCES Data By Major'!F114&amp;" } ,"</f>
-        <v>{ description: "Music", medianIncome: 40000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C116&amp;""", medianIncome: "&amp;'NCES Data By Major'!F116&amp;" } ,"</f>
+        <v>{ description: "Natural sciences", medianIncome: 48000 } ,</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C115&amp;""", medianIncome: "&amp;'NCES Data By Major'!F115&amp;" } ,"</f>
-        <v>{ description: "Natural sciences", medianIncome: 48000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C117&amp;""", medianIncome: "&amp;'NCES Data By Major'!F117&amp;" } ,"</f>
+        <v>{ description: "Neurobiology", medianIncome: 49000 } ,</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C116&amp;""", medianIncome: "&amp;'NCES Data By Major'!F116&amp;" } ,"</f>
-        <v>{ description: "Neurobiology", medianIncome: 49000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C118&amp;""", medianIncome: "&amp;'NCES Data By Major'!F118&amp;" } ,"</f>
+        <v>{ description: "Neuroscience", medianIncome: 49000 } ,</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C117&amp;""", medianIncome: "&amp;'NCES Data By Major'!F117&amp;" } ,"</f>
-        <v>{ description: "Neuroscience", medianIncome: 49000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C119&amp;""", medianIncome: "&amp;'NCES Data By Major'!F119&amp;" } ,"</f>
+        <v>{ description: "Nursing", medianIncome: 57000 } ,</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C118&amp;""", medianIncome: "&amp;'NCES Data By Major'!F118&amp;" } ,"</f>
-        <v>{ description: "Nursing", medianIncome: 57000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C120&amp;""", medianIncome: "&amp;'NCES Data By Major'!F120&amp;" } ,"</f>
+        <v>{ description: "Other", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C119&amp;""", medianIncome: "&amp;'NCES Data By Major'!F119&amp;" } ,"</f>
-        <v>{ description: "Other", medianIncome: 40000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C121&amp;""", medianIncome: "&amp;'NCES Data By Major'!F121&amp;" } ,"</f>
+        <v>{ description: "Paramedic Studies", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C120&amp;""", medianIncome: "&amp;'NCES Data By Major'!F120&amp;" } ,"</f>
-        <v>{ description: "Paramedic Studies", medianIncome: 42000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C122&amp;""", medianIncome: "&amp;'NCES Data By Major'!F122&amp;" } ,"</f>
+        <v>{ description: "Parks and Recreation", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C121&amp;""", medianIncome: "&amp;'NCES Data By Major'!F121&amp;" } ,"</f>
-        <v>{ description: "Parks and Recreation", medianIncome: 42000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C123&amp;""", medianIncome: "&amp;'NCES Data By Major'!F123&amp;" } ,"</f>
+        <v>{ description: "Pharmacology", medianIncome: 57000 } ,</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C122&amp;""", medianIncome: "&amp;'NCES Data By Major'!F122&amp;" } ,"</f>
-        <v>{ description: "Pharmacology", medianIncome: 57000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C124&amp;""", medianIncome: "&amp;'NCES Data By Major'!F124&amp;" } ,"</f>
+        <v>{ description: "Pharmacy", medianIncome: 57000 } ,</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C123&amp;""", medianIncome: "&amp;'NCES Data By Major'!F123&amp;" } ,"</f>
-        <v>{ description: "Pharmacy", medianIncome: 57000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C125&amp;""", medianIncome: "&amp;'NCES Data By Major'!F125&amp;" } ,"</f>
+        <v>{ description: "Philosophy", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C124&amp;""", medianIncome: "&amp;'NCES Data By Major'!F124&amp;" } ,"</f>
-        <v>{ description: "Philosophy", medianIncome: 42000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C126&amp;""", medianIncome: "&amp;'NCES Data By Major'!F126&amp;" } ,"</f>
+        <v>{ description: "Physical Chemistry", medianIncome: 48000 } ,</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C125&amp;""", medianIncome: "&amp;'NCES Data By Major'!F125&amp;" } ,"</f>
-        <v>{ description: "Physical Chemistry", medianIncome: 48000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C127&amp;""", medianIncome: "&amp;'NCES Data By Major'!F127&amp;" } ,"</f>
+        <v>{ description: "Physical Fitness", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C126&amp;""", medianIncome: "&amp;'NCES Data By Major'!F126&amp;" } ,"</f>
-        <v>{ description: "Physical Fitness", medianIncome: 42000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C128&amp;""", medianIncome: "&amp;'NCES Data By Major'!F128&amp;" } ,"</f>
+        <v>{ description: "Physical Sciences", medianIncome: 48000 } ,</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C127&amp;""", medianIncome: "&amp;'NCES Data By Major'!F127&amp;" } ,"</f>
-        <v>{ description: "Physical Sciences", medianIncome: 48000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C129&amp;""", medianIncome: "&amp;'NCES Data By Major'!F129&amp;" } ,"</f>
+        <v>{ description: "Physics", medianIncome: 48000 } ,</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C128&amp;""", medianIncome: "&amp;'NCES Data By Major'!F128&amp;" } ,"</f>
-        <v>{ description: "Physics", medianIncome: 48000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C130&amp;""", medianIncome: "&amp;'NCES Data By Major'!F130&amp;" } ,"</f>
+        <v>{ description: "Physiology", medianIncome: 49000 } ,</v>
       </c>
     </row>
     <row r="129" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B129" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C129&amp;""", medianIncome: "&amp;'NCES Data By Major'!F129&amp;" } ,"</f>
-        <v>{ description: "Physiology", medianIncome: 49000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C131&amp;""", medianIncome: "&amp;'NCES Data By Major'!F131&amp;" } ,"</f>
+        <v>{ description: "Political Science", medianIncome: 50000 } ,</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C130&amp;""", medianIncome: "&amp;'NCES Data By Major'!F130&amp;" } ,"</f>
-        <v>{ description: "Political Science", medianIncome: 50000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C132&amp;""", medianIncome: "&amp;'NCES Data By Major'!F132&amp;" } ,"</f>
+        <v>{ description: "Probabilities", medianIncome: 55000 } ,</v>
       </c>
     </row>
     <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C131&amp;""", medianIncome: "&amp;'NCES Data By Major'!F131&amp;" } ,"</f>
-        <v>{ description: "Probabilities", medianIncome: 55000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C133&amp;""", medianIncome: "&amp;'NCES Data By Major'!F133&amp;" } ,"</f>
+        <v>{ description: "Psychology", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C132&amp;""", medianIncome: "&amp;'NCES Data By Major'!F132&amp;" } ,"</f>
-        <v>{ description: "Psychology", medianIncome: 40000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C134&amp;""", medianIncome: "&amp;'NCES Data By Major'!F134&amp;" } ,"</f>
+        <v>{ description: "Public Administration", medianIncome: 45000 } ,</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B133" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C133&amp;""", medianIncome: "&amp;'NCES Data By Major'!F133&amp;" } ,"</f>
-        <v>{ description: "Public Administration", medianIncome: 45000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C135&amp;""", medianIncome: "&amp;'NCES Data By Major'!F135&amp;" } ,"</f>
+        <v>{ description: "Public Health", medianIncome: 51000 } ,</v>
       </c>
     </row>
     <row r="134" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B134" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C134&amp;""", medianIncome: "&amp;'NCES Data By Major'!F134&amp;" } ,"</f>
-        <v>{ description: "Public Health", medianIncome: 51000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C136&amp;""", medianIncome: "&amp;'NCES Data By Major'!F136&amp;" } ,"</f>
+        <v>{ description: "Public Policy", medianIncome: 45000 } ,</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C135&amp;""", medianIncome: "&amp;'NCES Data By Major'!F135&amp;" } ,"</f>
-        <v>{ description: "Public Policy", medianIncome: 45000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C137&amp;""", medianIncome: "&amp;'NCES Data By Major'!F137&amp;" } ,"</f>
+        <v>{ description: "Quantitative Finance", medianIncome: 64000 } ,</v>
       </c>
     </row>
     <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C136&amp;""", medianIncome: "&amp;'NCES Data By Major'!F136&amp;" } ,"</f>
-        <v>{ description: "Quantitative Finance", medianIncome: 64000 } ,</v>
+        <f>"{ description: """&amp;'NCES Data By Major'!C138&amp;""", medianIncome: "&amp;'NCES Data By Major'!F138&amp;" } ,"</f>
+        <v>{ description: "Radio", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C137&amp;""", medianIncome: "&amp;'NCES Data By Major'!F137&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C139&amp;""", medianIncome: "&amp;'NCES Data By Major'!F139&amp;" } ,"</f>
         <v>{ description: "Real Estate", medianIncome: 58000 } ,</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C138&amp;""", medianIncome: "&amp;'NCES Data By Major'!F138&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C140&amp;""", medianIncome: "&amp;'NCES Data By Major'!F140&amp;" } ,"</f>
         <v>{ description: "Religion", medianIncome: 35000 } ,</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C139&amp;""", medianIncome: "&amp;'NCES Data By Major'!F139&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C141&amp;""", medianIncome: "&amp;'NCES Data By Major'!F141&amp;" } ,"</f>
         <v>{ description: "Religious Studies", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C140&amp;""", medianIncome: "&amp;'NCES Data By Major'!F140&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C142&amp;""", medianIncome: "&amp;'NCES Data By Major'!F142&amp;" } ,"</f>
         <v>{ description: "Secondary School Education", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C141&amp;""", medianIncome: "&amp;'NCES Data By Major'!F141&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C143&amp;""", medianIncome: "&amp;'NCES Data By Major'!F143&amp;" } ,"</f>
         <v>{ description: "Social Sciences", medianIncome: 50000 } ,</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C142&amp;""", medianIncome: "&amp;'NCES Data By Major'!F142&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C144&amp;""", medianIncome: "&amp;'NCES Data By Major'!F144&amp;" } ,"</f>
         <v>{ description: "Social Studies", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B143" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C143&amp;""", medianIncome: "&amp;'NCES Data By Major'!F143&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C145&amp;""", medianIncome: "&amp;'NCES Data By Major'!F145&amp;" } ,"</f>
         <v>{ description: "Social Work", medianIncome: 38000 } ,</v>
       </c>
     </row>
@@ -20231,73 +20271,73 @@
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C144&amp;""", medianIncome: "&amp;'NCES Data By Major'!F144&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C146&amp;""", medianIncome: "&amp;'NCES Data By Major'!F146&amp;" } ,"</f>
         <v>{ description: "Sociology", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C145&amp;""", medianIncome: "&amp;'NCES Data By Major'!F145&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C147&amp;""", medianIncome: "&amp;'NCES Data By Major'!F147&amp;" } ,"</f>
         <v>{ description: "Sports Medicine", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C146&amp;""", medianIncome: "&amp;'NCES Data By Major'!F146&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C148&amp;""", medianIncome: "&amp;'NCES Data By Major'!F148&amp;" } ,"</f>
         <v>{ description: "Statistics", medianIncome: 66000 } ,</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C147&amp;""", medianIncome: "&amp;'NCES Data By Major'!F147&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C149&amp;""", medianIncome: "&amp;'NCES Data By Major'!F149&amp;" } ,"</f>
         <v>{ description: "Structural Engineering", medianIncome: 70000 } ,</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C148&amp;""", medianIncome: "&amp;'NCES Data By Major'!F148&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C150&amp;""", medianIncome: "&amp;'NCES Data By Major'!F150&amp;" } ,"</f>
         <v>{ description: "Studio Art", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C149&amp;""", medianIncome: "&amp;'NCES Data By Major'!F149&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C151&amp;""", medianIncome: "&amp;'NCES Data By Major'!F151&amp;" } ,"</f>
         <v>{ description: "Theatre", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C150&amp;""", medianIncome: "&amp;'NCES Data By Major'!F150&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C152&amp;""", medianIncome: "&amp;'NCES Data By Major'!F152&amp;" } ,"</f>
         <v>{ description: "Theology", medianIncome: 35000 } ,</v>
       </c>
     </row>
     <row r="152" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B152" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C151&amp;""", medianIncome: "&amp;'NCES Data By Major'!F151&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C153&amp;""", medianIncome: "&amp;'NCES Data By Major'!F153&amp;" } ,"</f>
         <v>{ description: "Transportation", medianIncome: 59000 } ,</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C152&amp;""", medianIncome: "&amp;'NCES Data By Major'!F152&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C154&amp;""", medianIncome: "&amp;'NCES Data By Major'!F154&amp;" } ,"</f>
         <v>{ description: "Travel and Leisure Services", medianIncome: 42000 } ,</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C153&amp;""", medianIncome: "&amp;'NCES Data By Major'!F153&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C155&amp;""", medianIncome: "&amp;'NCES Data By Major'!F155&amp;" } ,"</f>
         <v>{ description: "Undeclared", medianIncome: 40000 } ,</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C154&amp;""", medianIncome: "&amp;'NCES Data By Major'!F154&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C156&amp;""", medianIncome: "&amp;'NCES Data By Major'!F156&amp;" } ,"</f>
         <v>{ description: "Urban Studies and Planning", medianIncome: 41000 } ,</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" t="str">
-        <f>"{ description: """&amp;'NCES Data By Major'!C155&amp;""", medianIncome: "&amp;'NCES Data By Major'!F155&amp;" } ,"</f>
+        <f>"{ description: """&amp;'NCES Data By Major'!C157&amp;""", medianIncome: "&amp;'NCES Data By Major'!F157&amp;" } ,"</f>
         <v>{ description: "World Literature", medianIncome: 40000 } ,</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Super minor changes to language on the home page
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951FF101-019A-4968-8ACB-688F802DF337}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A64215-F540-4364-8FC8-81F02545C41E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4695" yWindow="3180" windowWidth="20910" windowHeight="11835" xr2:uid="{58DD74EF-95EE-4947-B358-20B5CBB4703D}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{58DD74EF-95EE-4947-B358-20B5CBB4703D}"/>
   </bookViews>
   <sheets>
     <sheet name="NCES Data By Major" sheetId="1" r:id="rId1"/>
@@ -6483,7 +6483,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6825,8 +6825,8 @@
   </sheetPr>
   <dimension ref="B2:F157"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A139" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A117" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9445,7 +9445,7 @@
         <v>119</v>
       </c>
       <c r="D155" s="9">
-        <v>0.09</v>
+        <v>0.15</v>
       </c>
       <c r="E155" s="10">
         <v>2.3E-2</v>

</xml_diff>

<commit_message>
Organization and refactoring for the institutions update to the website
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB89356-0065-4C03-A736-58E5F7592F2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACE1FDE-3932-4550-8707-3D9F57529C59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="300" windowWidth="17535" windowHeight="11430" activeTab="3" xr2:uid="{58DD74EF-95EE-4947-B358-20B5CBB4703D}"/>
+    <workbookView xWindow="1515" yWindow="90" windowWidth="17535" windowHeight="11430" activeTab="3" xr2:uid="{58DD74EF-95EE-4947-B358-20B5CBB4703D}"/>
   </bookViews>
   <sheets>
     <sheet name="NCES Data By Major" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="2118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="2119">
   <si>
     <t>Agriculture</t>
   </si>
@@ -6410,6 +6410,9 @@
   </si>
   <si>
     <t>AverageLoanDebtAtGraduation</t>
+  </si>
+  <si>
+    <t>CohortDefaultRate</t>
   </si>
 </sst>
 </file>
@@ -6419,9 +6422,9 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6456,12 +6459,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -6579,8 +6576,8 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -20458,10 +20455,10 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20471,9 +20468,10 @@
     <col min="3" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>2105</v>
       </c>
@@ -20498,8 +20496,11 @@
       <c r="H1" s="12" t="s">
         <v>2110</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="12" t="s">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2111</v>
       </c>
@@ -20528,8 +20529,11 @@
         <f>H5*2</f>
         <v>0.12</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="15">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2111</v>
       </c>
@@ -20558,8 +20562,11 @@
         <f t="shared" ref="H3:H4" si="3">H6*2</f>
         <v>0.06</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="15">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2111</v>
       </c>
@@ -20588,8 +20595,11 @@
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="15">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2115</v>
       </c>
@@ -20614,8 +20624,11 @@
       <c r="H5" s="15">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="15">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2115</v>
       </c>
@@ -20640,8 +20653,11 @@
       <c r="H6" s="15">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="15">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2115</v>
       </c>
@@ -20665,6 +20681,9 @@
       </c>
       <c r="H7" s="15">
         <v>0.1</v>
+      </c>
+      <c r="I7" s="15">
+        <v>0.22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to website inputs
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.WebApi\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dar Vadar\Desktop\EduSafe Repo\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACE1FDE-3932-4550-8707-3D9F57529C59}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA12AADC-D1FF-4BC9-BD73-81E21F0A1487}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="90" windowWidth="17535" windowHeight="11430" activeTab="3" xr2:uid="{58DD74EF-95EE-4947-B358-20B5CBB4703D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{58DD74EF-95EE-4947-B358-20B5CBB4703D}"/>
   </bookViews>
   <sheets>
     <sheet name="NCES Data By Major" sheetId="1" r:id="rId1"/>
@@ -35,24 +35,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={5B50B68C-70DF-41F3-8EDB-6FEA9E0BA90D}</author>
-  </authors>
-  <commentList>
-    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{5B50B68C-70DF-41F3-8EDB-6FEA9E0BA90D}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    All these blue numbers are basically made up. Definitely need Sharon to think through how to parameterize these better.</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6609,9 +6591,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Matthew Moore" id="{3924B701-B7D2-4B05-A6A9-AEE341F8BE4B}" userId="2877da6b73c883a8" providerId="Windows Live"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6909,14 +6889,6 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="H2" dT="2019-07-31T14:51:00.75" personId="{3924B701-B7D2-4B05-A6A9-AEE341F8BE4B}" id="{5B50B68C-70DF-41F3-8EDB-6FEA9E0BA90D}">
-    <text>All these blue numbers are basically made up. Definitely need Sharon to think through how to parameterize these better.</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288A81B0-662D-4677-8BAF-C98B4ED9498B}">
   <sheetPr>
@@ -6925,7 +6897,7 @@
   <dimension ref="B2:F157"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20451,14 +20423,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFA74A12-6BA9-461B-86D7-F00F32E7CA93}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFA74A12-6BA9-461B-86D7-F00F32E7CA93}">
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20522,12 +20494,12 @@
         <v>0.25</v>
       </c>
       <c r="G2" s="14">
-        <f>(G5/F5)*F2</f>
+        <f t="shared" ref="G2:G4" si="0">(G5/F5)*F2</f>
         <v>0.27272727272727271</v>
       </c>
       <c r="H2" s="13">
-        <f>H5*2</f>
-        <v>0.12</v>
+        <f>G2*H5/G5</f>
+        <v>2.7272727272727271E-2</v>
       </c>
       <c r="I2" s="15">
         <v>0.21</v>
@@ -20541,26 +20513,26 @@
         <v>2113</v>
       </c>
       <c r="C3" s="17">
-        <f t="shared" ref="C3:C4" si="0">C6/2</f>
+        <f t="shared" ref="C3:C4" si="1">C6/2</f>
         <v>16300</v>
       </c>
       <c r="D3" s="16">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E3" s="14">
-        <f t="shared" ref="E3:E4" si="1">(E6/F6)*F3</f>
+        <f t="shared" ref="E3:E4" si="2">(E6/F6)*F3</f>
         <v>0.52312499999999995</v>
       </c>
       <c r="F3" s="15">
         <v>0.62</v>
       </c>
       <c r="G3" s="14">
-        <f t="shared" ref="G3:G4" si="2">(G6/F6)*F3</f>
+        <f t="shared" si="0"/>
         <v>0.63937500000000003</v>
       </c>
       <c r="H3" s="13">
-        <f t="shared" ref="H3:H4" si="3">H6*2</f>
-        <v>0.06</v>
+        <f t="shared" ref="H3:H4" si="3">G3*H6/G6</f>
+        <v>2.9062499999999998E-2</v>
       </c>
       <c r="I3" s="15">
         <v>0.14000000000000001</v>
@@ -20574,26 +20546,26 @@
         <v>2114</v>
       </c>
       <c r="C4" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19750</v>
       </c>
       <c r="D4" s="16">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E4" s="14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.44947368421052636</v>
       </c>
       <c r="F4" s="15">
         <v>0.61</v>
       </c>
       <c r="G4" s="14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>0.67421052631578937</v>
       </c>
       <c r="H4" s="13">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.32105263157894731</v>
       </c>
       <c r="I4" s="15">
         <v>0.21</v>
@@ -20689,6 +20661,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change the 2 year graduation rate logic
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dar Vadar\Desktop\EduSafe Repo\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA12AADC-D1FF-4BC9-BD73-81E21F0A1487}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6279FD5-7DFC-4CBF-98B3-5AEA7AD2CB43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{58DD74EF-95EE-4947-B358-20B5CBB4703D}"/>
   </bookViews>
@@ -6549,9 +6549,6 @@
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6560,6 +6557,9 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6588,10 +6588,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20430,7 +20426,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20479,29 +20475,29 @@
       <c r="B2" t="s">
         <v>2112</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="16">
         <f>C5/2</f>
         <v>13450</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E2" s="14">
-        <f>(E5/F5)*F2</f>
-        <v>0.16818181818181815</v>
-      </c>
-      <c r="F2" s="15">
+      <c r="E2" s="13">
+        <f>E5/F5*F2</f>
+        <v>0.15416666666666665</v>
+      </c>
+      <c r="F2" s="13">
+        <f>F5/G5*G2</f>
+        <v>0.22916666666666669</v>
+      </c>
+      <c r="G2" s="18">
         <v>0.25</v>
-      </c>
-      <c r="G2" s="14">
-        <f t="shared" ref="G2:G4" si="0">(G5/F5)*F2</f>
-        <v>0.27272727272727271</v>
       </c>
       <c r="H2" s="13">
         <f>G2*H5/G5</f>
-        <v>2.7272727272727271E-2</v>
-      </c>
-      <c r="I2" s="15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="I2" s="14">
         <v>0.21</v>
       </c>
     </row>
@@ -20512,29 +20508,29 @@
       <c r="B3" t="s">
         <v>2113</v>
       </c>
-      <c r="C3" s="17">
-        <f t="shared" ref="C3:C4" si="1">C6/2</f>
+      <c r="C3" s="16">
+        <f t="shared" ref="C3:C4" si="0">C6/2</f>
         <v>16300</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E3" s="14">
-        <f t="shared" ref="E3:E4" si="2">(E6/F6)*F3</f>
-        <v>0.52312499999999995</v>
-      </c>
-      <c r="F3" s="15">
+      <c r="E3" s="13">
+        <f t="shared" ref="E3:F4" si="1">E6/F6*F3</f>
+        <v>0.50727272727272721</v>
+      </c>
+      <c r="F3" s="13">
+        <f t="shared" si="1"/>
+        <v>0.6012121212121212</v>
+      </c>
+      <c r="G3" s="18">
         <v>0.62</v>
       </c>
-      <c r="G3" s="14">
-        <f t="shared" si="0"/>
-        <v>0.63937500000000003</v>
-      </c>
       <c r="H3" s="13">
-        <f t="shared" ref="H3:H4" si="3">G3*H6/G6</f>
-        <v>2.9062499999999998E-2</v>
-      </c>
-      <c r="I3" s="15">
+        <f t="shared" ref="H3:H4" si="2">G3*H6/G6</f>
+        <v>2.8181818181818179E-2</v>
+      </c>
+      <c r="I3" s="14">
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -20545,29 +20541,29 @@
       <c r="B4" t="s">
         <v>2114</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="16">
+        <f t="shared" si="0"/>
+        <v>19750</v>
+      </c>
+      <c r="D4" s="15">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E4" s="13">
         <f t="shared" si="1"/>
-        <v>19750</v>
-      </c>
-      <c r="D4" s="16">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="E4" s="14">
+        <v>0.40666666666666668</v>
+      </c>
+      <c r="F4" s="13">
+        <f t="shared" si="1"/>
+        <v>0.5519047619047619</v>
+      </c>
+      <c r="G4" s="18">
+        <v>0.61</v>
+      </c>
+      <c r="H4" s="13">
         <f t="shared" si="2"/>
-        <v>0.44947368421052636</v>
-      </c>
-      <c r="F4" s="15">
-        <v>0.61</v>
-      </c>
-      <c r="G4" s="14">
-        <f t="shared" si="0"/>
-        <v>0.67421052631578937</v>
-      </c>
-      <c r="H4" s="13">
-        <f t="shared" si="3"/>
-        <v>0.32105263157894731</v>
-      </c>
-      <c r="I4" s="15">
+        <v>0.2904761904761905</v>
+      </c>
+      <c r="I4" s="14">
         <v>0.21</v>
       </c>
     </row>
@@ -20578,25 +20574,25 @@
       <c r="B5" t="s">
         <v>2112</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>26900</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>0.37</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="14">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="14">
         <v>0.6</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <v>0.06</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="14">
         <v>0.09</v>
       </c>
     </row>
@@ -20607,25 +20603,25 @@
       <c r="B6" t="s">
         <v>2113</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>32600</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="15">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>0.54</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="14">
         <v>0.64</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="14">
         <v>0.66</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>0.03</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="14">
         <v>0.08</v>
       </c>
     </row>
@@ -20636,25 +20632,25 @@
       <c r="B7" t="s">
         <v>2114</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <v>39500</v>
       </c>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="14">
         <v>0.19</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="14">
         <v>0.21</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <v>0.1</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I7" s="14">
         <v>0.22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed links from files and ensured that all tests are passing
</commit_message>
<xml_diff>
--- a/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
+++ b/EduSafe.WebApi/App_Data/EduSafe-Website-College-Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dar Vadar\Desktop\EduSafe Repo\edusafe\EduSafe.WebApi\App_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew M\edusafe\EduSafe.WebApi\App_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6279FD5-7DFC-4CBF-98B3-5AEA7AD2CB43}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BADEB21-9FD4-423F-A1AA-ED7499965277}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{58DD74EF-95EE-4947-B358-20B5CBB4703D}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="3" xr2:uid="{58DD74EF-95EE-4947-B358-20B5CBB4703D}"/>
   </bookViews>
   <sheets>
     <sheet name="NCES Data By Major" sheetId="1" r:id="rId1"/>
@@ -6520,7 +6520,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -6558,6 +6558,9 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -20426,7 +20429,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20483,18 +20486,18 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E2" s="13">
-        <f>E5/F5*F2</f>
-        <v>0.15416666666666665</v>
-      </c>
-      <c r="F2" s="13">
-        <f>F5/G5*G2</f>
-        <v>0.22916666666666669</v>
-      </c>
-      <c r="G2" s="18">
+        <f>E5/G5*F2</f>
+        <v>0.15416666666666667</v>
+      </c>
+      <c r="F2" s="18">
         <v>0.25</v>
       </c>
+      <c r="G2" s="19">
+        <f>G5/F5*F2</f>
+        <v>0.27272727272727271</v>
+      </c>
       <c r="H2" s="13">
-        <f>G2*H5/G5</f>
+        <f>F2*H5/G5</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I2" s="14">
@@ -20516,18 +20519,18 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="E3" s="13">
-        <f t="shared" ref="E3:F4" si="1">E6/F6*F3</f>
-        <v>0.50727272727272721</v>
-      </c>
-      <c r="F3" s="13">
-        <f t="shared" si="1"/>
-        <v>0.6012121212121212</v>
-      </c>
-      <c r="G3" s="18">
+        <f t="shared" ref="E3:E4" si="1">E6/G6*F3</f>
+        <v>0.50727272727272732</v>
+      </c>
+      <c r="F3" s="18">
         <v>0.62</v>
       </c>
+      <c r="G3" s="19">
+        <f t="shared" ref="G3:G4" si="2">G6/F6*F3</f>
+        <v>0.63937500000000003</v>
+      </c>
       <c r="H3" s="13">
-        <f t="shared" ref="H3:H4" si="2">G3*H6/G6</f>
+        <f t="shared" ref="H3:H4" si="3">F3*H6/G6</f>
         <v>2.8181818181818179E-2</v>
       </c>
       <c r="I3" s="14">
@@ -20552,15 +20555,15 @@
         <f t="shared" si="1"/>
         <v>0.40666666666666668</v>
       </c>
-      <c r="F4" s="13">
-        <f t="shared" si="1"/>
-        <v>0.5519047619047619</v>
-      </c>
-      <c r="G4" s="18">
+      <c r="F4" s="18">
         <v>0.61</v>
       </c>
+      <c r="G4" s="19">
+        <f t="shared" si="2"/>
+        <v>0.67421052631578937</v>
+      </c>
       <c r="H4" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2904761904761905</v>
       </c>
       <c r="I4" s="14">

</xml_diff>